<commit_message>
Actualización de la documentación del procesado inicial del dataset. Actualización de la comprensión del negocio, y tabla ODS.
</commit_message>
<xml_diff>
--- a/data/ODS.xlsx
+++ b/data/ODS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleja\Documents\Universidad\2º Curso\1er Cuatrimestre\AEDV\proyecto personal\ProyectoPersonal_AEDV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleja\Documents\Universidad\2º Curso\1er Cuatrimestre\AEDV\proyecto personal\ProyectoPersonal_AEDV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D9B48D-8AD6-4F44-9AC0-9781BF9DBC28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F53F0F8-764D-4F4C-961A-398E1E90C313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7355BA2D-9C48-415E-81BC-138F08BEB434}"/>
   </bookViews>
@@ -140,8 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +480,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,7 +509,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -516,7 +517,7 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -524,7 +525,7 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -540,7 +541,7 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -642,5 +643,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>